<commit_message>
added by sheet exporting
</commit_message>
<xml_diff>
--- a/Try.xlsx
+++ b/Try.xlsx
@@ -7,7 +7,11 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="TRY" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Slice_Rows_First3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Filtered_Age&gt;25" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Loc_Slice" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -572,4 +576,386 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Occupation</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Score</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Alice</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>24</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Data Analyst</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Bob</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>30</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Engineer</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Charlie</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>22</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Teacher</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Diana</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>28</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Designer</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Evan</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>35</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Manager</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Occupation</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Score</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Alice</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>24</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Data Analyst</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Bob</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>30</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Engineer</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Charlie</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>22</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Teacher</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Occupation</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Score</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Bob</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>30</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Engineer</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Diana</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>28</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Designer</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Evan</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>35</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Manager</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Score</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Bob</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Charlie</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Diana</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>